<commit_message>
A couple supply kit translations were incomplete
</commit_message>
<xml_diff>
--- a/translations/admin-strings-all.xlsx
+++ b/translations/admin-strings-all.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="552">
   <si>
     <t>English</t>
   </si>
@@ -2412,28 +2412,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Es probable que ya tenga la mayoría de los elementos necesarios para su &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/FamilyDisasterSuppliesKitRedCross.pdf" target=_blank&gt;kit de suministros familiares&lt;/a&gt;. Averigüe qué más agregar y organícese antes del próximo evento. También es buena idea tener un kit de emergencia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/carkit.pdf" target=_blank&gt;de automóvil&lt;/a&gt;.</t>
-    </r>
-  </si>
-  <si>
     <t>Vietnamese</t>
   </si>
   <si>
@@ -2692,12 +2670,6 @@
     <t>Điều Gì Có Thể Xảy Ra</t>
   </si>
   <si>
-    <t>Có vẻ như bạn đã có hầu hết các vật dụng cần thiết cho &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/FamilyDisasterSuppliesKitRedCross.pdf" target=_blank&gt;bộ dụng cụ khẩn cấp cho gia đình&lt;/a&gt; rồi. Tìm hiểu về các vật dụng nào cần bổ sung và sắp xếp vật dụng đó trước khi sự cố tiếp theo xảy ra. Một ý tưởng cũng rất hữu ích là có sẵn một</t>
-  </si>
-  <si>
-    <t>&lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/carkit.pdf" target=_blank&gt;bộ dụng cụ khẩn cấp trên xe&lt;/a&gt;.</t>
-  </si>
-  <si>
     <t>It's likely you have most items you need for your &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/FamilyDisasterSuppliesKitRedCross.pdf" target=_blank&gt;family supply kit&lt;/a&gt; already. Find out what else to add and get it organized before the next event hits. It's also a good idea to have an emergency &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/carkit.pdf" target=_blank&gt;car kit&lt;/a&gt;.</t>
   </si>
   <si>
@@ -3611,6 +3583,12 @@
   </si>
   <si>
     <t>Trang web của &lt;a href="http://www.seattle.gov/emergency-management" target="_blank"&gt;VP Quản Lý Trường Hợp Khẩn Cấp Seattle&lt;/a&gt; có rất nhiều tài nguyên để tìm hiểu thêm.</t>
+  </si>
+  <si>
+    <t>Es probable que ya tenga la mayoría de los elementos necesarios para su &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/FamilyDisasterSuppliesKitRedCross.pdf" target=_blank&gt;kit de suministros familiares&lt;/a&gt;. Averigüe qué más agregar y organícese antes del próximo evento. También es buena idea tener un kit de emergencia &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/carkit.pdf" target=_blank&gt;de automóvil&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Có vẻ như bạn đã có hầu hết các vật dụng cần thiết cho &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/FamilyDisasterSuppliesKitRedCross.pdf" target=_blank&gt;bộ dụng cụ khẩn cấp cho gia đình&lt;/a&gt; rồi. Tìm hiểu về các vật dụng nào cần bổ sung và sắp xếp vật dụng đó trước khi sự cố tiếp theo xảy ra. Một ý tưởng cũng rất hữu ích là có sẵn một &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/carkit.pdf" target=_blank&gt;bộ dụng cụ khẩn cấp trên xe&lt;/a&gt;.</t>
   </si>
 </sst>
 </file>
@@ -4056,21 +4034,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="75.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="61" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" style="9"/>
-    <col min="4" max="4" width="75.6640625" style="2"/>
-    <col min="5" max="5" width="75.6640625" style="5"/>
-    <col min="6" max="6" width="75.6640625" style="18"/>
+    <col min="3" max="3" width="10.83203125" style="9"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="10.83203125" style="5"/>
+    <col min="6" max="6" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4087,10 +4065,10 @@
         <v>263</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="81" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -4098,7 +4076,7 @@
         <v>172</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -4107,10 +4085,10 @@
         <v>264</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="65" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
@@ -4118,7 +4096,7 @@
         <v>173</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -4127,10 +4105,10 @@
         <v>265</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="97" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
@@ -4138,7 +4116,7 @@
         <v>174</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -4147,10 +4125,10 @@
         <v>266</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="49" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -4158,7 +4136,7 @@
         <v>175</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>9</v>
@@ -4167,10 +4145,10 @@
         <v>267</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>10</v>
       </c>
@@ -4178,7 +4156,7 @@
         <v>176</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -4187,10 +4165,10 @@
         <v>268</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="81" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
@@ -4198,7 +4176,7 @@
         <v>177</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
@@ -4207,10 +4185,10 @@
         <v>269</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="65" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
@@ -4218,7 +4196,7 @@
         <v>178</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
@@ -4227,10 +4205,10 @@
         <v>270</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="80" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
@@ -4238,7 +4216,7 @@
         <v>179</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>17</v>
@@ -4247,10 +4225,10 @@
         <v>271</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="65" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>18</v>
       </c>
@@ -4258,7 +4236,7 @@
         <v>180</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>19</v>
@@ -4267,10 +4245,10 @@
         <v>272</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="65" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -4278,7 +4256,7 @@
         <v>181</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
@@ -4287,10 +4265,10 @@
         <v>273</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="112" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>22</v>
       </c>
@@ -4298,7 +4276,7 @@
         <v>182</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>23</v>
@@ -4307,10 +4285,10 @@
         <v>274</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="49" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>24</v>
       </c>
@@ -4318,7 +4296,7 @@
         <v>183</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>25</v>
@@ -4327,10 +4305,10 @@
         <v>275</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="64" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>26</v>
       </c>
@@ -4338,7 +4316,7 @@
         <v>184</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>27</v>
@@ -4347,10 +4325,10 @@
         <v>276</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>28</v>
       </c>
@@ -4358,7 +4336,7 @@
         <v>185</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>29</v>
@@ -4367,10 +4345,10 @@
         <v>277</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="80" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>30</v>
       </c>
@@ -4387,10 +4365,10 @@
         <v>278</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="81" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>32</v>
       </c>
@@ -4398,7 +4376,7 @@
         <v>187</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>33</v>
@@ -4407,10 +4385,10 @@
         <v>279</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="112" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>34</v>
       </c>
@@ -4418,7 +4396,7 @@
         <v>188</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>35</v>
@@ -4427,30 +4405,30 @@
         <v>280</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>527</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>528</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>530</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="F19" s="19" t="s">
         <v>531</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>532</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>534</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" ht="64" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>36</v>
       </c>
@@ -4458,7 +4436,7 @@
         <v>189</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>37</v>
@@ -4467,30 +4445,30 @@
         <v>281</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
+        <v>532</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>533</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>534</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="F21" s="19" t="s">
         <v>537</v>
       </c>
-      <c r="C21" s="16" t="s">
-        <v>538</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>539</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>540</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" ht="48" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>38</v>
       </c>
@@ -4498,7 +4476,7 @@
         <v>190</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>39</v>
@@ -4507,30 +4485,30 @@
         <v>282</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="256" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
+        <v>538</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>539</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>540</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>542</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="F23" s="19" t="s">
         <v>543</v>
       </c>
-      <c r="C23" s="16" t="s">
-        <v>544</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>545</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>546</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6" ht="128" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>40</v>
       </c>
@@ -4538,7 +4516,7 @@
         <v>191</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>41</v>
@@ -4547,30 +4525,30 @@
         <v>283</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="368" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
+        <v>544</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>545</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>546</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>548</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="F25" s="19" t="s">
         <v>549</v>
       </c>
-      <c r="C25" s="16" t="s">
-        <v>550</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>551</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>552</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>42</v>
       </c>
@@ -4578,7 +4556,7 @@
         <v>192</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>43</v>
@@ -4587,10 +4565,10 @@
         <v>284</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="320" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>44</v>
       </c>
@@ -4598,7 +4576,7 @@
         <v>193</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>45</v>
@@ -4607,10 +4585,10 @@
         <v>285</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="368" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>46</v>
       </c>
@@ -4618,7 +4596,7 @@
         <v>194</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>47</v>
@@ -4627,10 +4605,10 @@
         <v>286</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="96" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>48</v>
       </c>
@@ -4638,7 +4616,7 @@
         <v>195</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>49</v>
@@ -4647,10 +4625,10 @@
         <v>287</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="108" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>50</v>
       </c>
@@ -4658,7 +4636,7 @@
         <v>196</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>51</v>
@@ -4667,10 +4645,10 @@
         <v>288</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>52</v>
       </c>
@@ -4678,7 +4656,7 @@
         <v>197</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>53</v>
@@ -4687,10 +4665,10 @@
         <v>289</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="108" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>54</v>
       </c>
@@ -4698,7 +4676,7 @@
         <v>198</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>55</v>
@@ -4707,10 +4685,10 @@
         <v>290</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="144" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>56</v>
       </c>
@@ -4718,7 +4696,7 @@
         <v>199</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>57</v>
@@ -4727,10 +4705,10 @@
         <v>291</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="304" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>58</v>
       </c>
@@ -4738,7 +4716,7 @@
         <v>200</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>59</v>
@@ -4747,10 +4725,10 @@
         <v>292</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="48" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="368" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>60</v>
       </c>
@@ -4758,7 +4736,7 @@
         <v>201</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>61</v>
@@ -4767,10 +4745,10 @@
         <v>293</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="97" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>62</v>
       </c>
@@ -4778,7 +4756,7 @@
         <v>202</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>63</v>
@@ -4787,10 +4765,10 @@
         <v>294</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>64</v>
       </c>
@@ -4798,7 +4776,7 @@
         <v>203</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>65</v>
@@ -4807,10 +4785,10 @@
         <v>295</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>66</v>
       </c>
@@ -4818,7 +4796,7 @@
         <v>204</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>67</v>
@@ -4827,10 +4805,10 @@
         <v>296</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="32" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="192" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>68</v>
       </c>
@@ -4838,7 +4816,7 @@
         <v>205</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>69</v>
@@ -4847,10 +4825,10 @@
         <v>297</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="384" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>70</v>
       </c>
@@ -4867,10 +4845,10 @@
         <v>298</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="224" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>72</v>
       </c>
@@ -4887,10 +4865,10 @@
         <v>299</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>74</v>
       </c>
@@ -4898,7 +4876,7 @@
         <v>208</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>75</v>
@@ -4907,10 +4885,10 @@
         <v>300</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="176" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>76</v>
       </c>
@@ -4918,7 +4896,7 @@
         <v>209</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>77</v>
@@ -4927,10 +4905,10 @@
         <v>301</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="400" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>78</v>
       </c>
@@ -4938,7 +4916,7 @@
         <v>210</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>79</v>
@@ -4947,10 +4925,10 @@
         <v>302</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="72" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>80</v>
       </c>
@@ -4958,7 +4936,7 @@
         <v>211</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>81</v>
@@ -4967,10 +4945,10 @@
         <v>303</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="304" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>82</v>
       </c>
@@ -4978,7 +4956,7 @@
         <v>212</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>83</v>
@@ -4987,10 +4965,10 @@
         <v>304</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="80" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>84</v>
       </c>
@@ -4998,7 +4976,7 @@
         <v>213</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>85</v>
@@ -5007,10 +4985,10 @@
         <v>305</v>
       </c>
       <c r="F47" s="17" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="144" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>86</v>
       </c>
@@ -5018,7 +4996,7 @@
         <v>214</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>87</v>
@@ -5027,10 +5005,10 @@
         <v>306</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="80" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>88</v>
       </c>
@@ -5038,7 +5016,7 @@
         <v>215</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>89</v>
@@ -5047,10 +5025,10 @@
         <v>307</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>90</v>
       </c>
@@ -5058,7 +5036,7 @@
         <v>216</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>91</v>
@@ -5067,10 +5045,10 @@
         <v>308</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="304" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>92</v>
       </c>
@@ -5078,7 +5056,7 @@
         <v>217</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>93</v>
@@ -5087,10 +5065,10 @@
         <v>309</v>
       </c>
       <c r="F51" s="17" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="48" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="400" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>94</v>
       </c>
@@ -5098,7 +5076,7 @@
         <v>218</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>95</v>
@@ -5107,10 +5085,10 @@
         <v>310</v>
       </c>
       <c r="F52" s="17" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="96" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>96</v>
       </c>
@@ -5118,7 +5096,7 @@
         <v>219</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>97</v>
@@ -5127,10 +5105,10 @@
         <v>311</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="108" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>98</v>
       </c>
@@ -5138,7 +5116,7 @@
         <v>220</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>99</v>
@@ -5147,10 +5125,10 @@
         <v>312</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="126" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>100</v>
       </c>
@@ -5158,7 +5136,7 @@
         <v>221</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>101</v>
@@ -5167,10 +5145,10 @@
         <v>313</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="97" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>102</v>
       </c>
@@ -5178,7 +5156,7 @@
         <v>222</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>103</v>
@@ -5187,10 +5165,10 @@
         <v>314</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="108" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>104</v>
       </c>
@@ -5198,7 +5176,7 @@
         <v>223</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>105</v>
@@ -5207,10 +5185,10 @@
         <v>315</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>106</v>
       </c>
@@ -5218,7 +5196,7 @@
         <v>224</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>107</v>
@@ -5227,10 +5205,10 @@
         <v>316</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="128" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>108</v>
       </c>
@@ -5247,10 +5225,10 @@
         <v>317</v>
       </c>
       <c r="F59" s="17" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="126" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>110</v>
       </c>
@@ -5258,7 +5236,7 @@
         <v>226</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>111</v>
@@ -5267,10 +5245,10 @@
         <v>318</v>
       </c>
       <c r="F60" s="17" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="49" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="400" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>112</v>
       </c>
@@ -5278,7 +5256,7 @@
         <v>227</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>113</v>
@@ -5287,10 +5265,10 @@
         <v>319</v>
       </c>
       <c r="F61" s="17" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>114</v>
       </c>
@@ -5298,7 +5276,7 @@
         <v>228</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>115</v>
@@ -5307,10 +5285,10 @@
         <v>320</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="352" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>116</v>
       </c>
@@ -5318,7 +5296,7 @@
         <v>229</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>117</v>
@@ -5327,10 +5305,10 @@
         <v>321</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>118</v>
       </c>
@@ -5338,7 +5316,7 @@
         <v>230</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>119</v>
@@ -5347,10 +5325,10 @@
         <v>322</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>120</v>
       </c>
@@ -5358,7 +5336,7 @@
         <v>231</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>121</v>
@@ -5367,10 +5345,10 @@
         <v>323</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>122</v>
       </c>
@@ -5378,7 +5356,7 @@
         <v>232</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>123</v>
@@ -5387,10 +5365,10 @@
         <v>324</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="80" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>124</v>
       </c>
@@ -5398,7 +5376,7 @@
         <v>233</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>125</v>
@@ -5407,10 +5385,10 @@
         <v>325</v>
       </c>
       <c r="F67" s="17" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>126</v>
       </c>
@@ -5418,7 +5396,7 @@
         <v>234</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>127</v>
@@ -5427,10 +5405,10 @@
         <v>326</v>
       </c>
       <c r="F68" s="17" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="108" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>128</v>
       </c>
@@ -5438,7 +5416,7 @@
         <v>235</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>129</v>
@@ -5447,10 +5425,10 @@
         <v>327</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="80" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>130</v>
       </c>
@@ -5458,7 +5436,7 @@
         <v>236</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>131</v>
@@ -5467,10 +5445,10 @@
         <v>328</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="80" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>132</v>
       </c>
@@ -5478,7 +5456,7 @@
         <v>237</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>133</v>
@@ -5487,10 +5465,10 @@
         <v>329</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>134</v>
       </c>
@@ -5498,7 +5476,7 @@
         <v>238</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>135</v>
@@ -5507,10 +5485,10 @@
         <v>330</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>136</v>
       </c>
@@ -5518,7 +5496,7 @@
         <v>239</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>137</v>
@@ -5527,10 +5505,10 @@
         <v>331</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="400" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>138</v>
       </c>
@@ -5538,7 +5516,7 @@
         <v>240</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>139</v>
@@ -5547,10 +5525,10 @@
         <v>332</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>140</v>
       </c>
@@ -5558,7 +5536,7 @@
         <v>241</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>141</v>
@@ -5567,10 +5545,10 @@
         <v>333</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="48" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>142</v>
       </c>
@@ -5578,7 +5556,7 @@
         <v>242</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>143</v>
@@ -5587,10 +5565,10 @@
         <v>334</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>144</v>
       </c>
@@ -5598,7 +5576,7 @@
         <v>243</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>145</v>
@@ -5607,10 +5585,10 @@
         <v>335</v>
       </c>
       <c r="F77" s="17" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>146</v>
       </c>
@@ -5618,7 +5596,7 @@
         <v>244</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>147</v>
@@ -5627,10 +5605,10 @@
         <v>336</v>
       </c>
       <c r="F78" s="17" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>148</v>
       </c>
@@ -5638,7 +5616,7 @@
         <v>245</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>149</v>
@@ -5647,10 +5625,10 @@
         <v>337</v>
       </c>
       <c r="F79" s="17" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="32" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>150</v>
       </c>
@@ -5658,7 +5636,7 @@
         <v>246</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>151</v>
@@ -5667,10 +5645,10 @@
         <v>338</v>
       </c>
       <c r="F80" s="17" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>152</v>
       </c>
@@ -5678,7 +5656,7 @@
         <v>247</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>153</v>
@@ -5687,10 +5665,10 @@
         <v>339</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="48" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="368" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>154</v>
       </c>
@@ -5698,7 +5676,7 @@
         <v>248</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>155</v>
@@ -5707,10 +5685,10 @@
         <v>340</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="32" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="192" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>156</v>
       </c>
@@ -5718,7 +5696,7 @@
         <v>249</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>157</v>
@@ -5727,10 +5705,10 @@
         <v>341</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="65" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>158</v>
       </c>
@@ -5738,7 +5716,7 @@
         <v>250</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>159</v>
@@ -5747,10 +5725,10 @@
         <v>342</v>
       </c>
       <c r="F84" s="17" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="112" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>160</v>
       </c>
@@ -5758,7 +5736,7 @@
         <v>251</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>161</v>
@@ -5767,10 +5745,10 @@
         <v>343</v>
       </c>
       <c r="F85" s="17" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="48" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="336" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>162</v>
       </c>
@@ -5787,10 +5765,10 @@
         <v>344</v>
       </c>
       <c r="F86" s="17" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="396" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>164</v>
       </c>
@@ -5798,19 +5776,19 @@
         <v>253</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>345</v>
       </c>
       <c r="F87" s="17" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="48" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>165</v>
       </c>
@@ -5818,7 +5796,7 @@
         <v>254</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>166</v>
@@ -5827,10 +5805,10 @@
         <v>346</v>
       </c>
       <c r="F88" s="17" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="49" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>167</v>
       </c>
@@ -5838,7 +5816,7 @@
         <v>255</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>168</v>
@@ -5847,10 +5825,10 @@
         <v>347</v>
       </c>
       <c r="F89" s="17" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>169</v>
       </c>
@@ -5858,7 +5836,7 @@
         <v>256</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>170</v>
@@ -5867,59 +5845,53 @@
         <v>348</v>
       </c>
       <c r="F90" s="17" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="B91" s="10" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" ht="144" x14ac:dyDescent="0.25">
-      <c r="A91" s="9" t="s">
-        <v>439</v>
-      </c>
-      <c r="B91" s="10" t="s">
-        <v>440</v>
-      </c>
       <c r="C91" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="E91" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="F91" s="19" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="A92" s="11" t="s">
+        <v>437</v>
+      </c>
+      <c r="B92" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>520</v>
+      </c>
+      <c r="D92" s="13" t="s">
         <v>523</v>
       </c>
-      <c r="D91" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="F91" s="17" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A92" s="11" t="s">
-        <v>441</v>
-      </c>
-      <c r="B92" s="12" t="s">
-        <v>442</v>
-      </c>
-      <c r="C92" s="13" t="s">
+      <c r="E92" s="13" t="s">
         <v>524</v>
       </c>
-      <c r="D92" s="13" t="s">
-        <v>527</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="F92" s="17" t="s">
-        <v>438</v>
+      <c r="F92" s="11" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A93" s="11"/>
       <c r="B93" s="12"/>
       <c r="C93" s="13"/>
-      <c r="E93" s="13" t="s">
-        <v>528</v>
-      </c>
-      <c r="F93" s="11" t="s">
-        <v>529</v>
-      </c>
     </row>
     <row r="94" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A94" s="11"/>

</xml_diff>

<commit_message>
Fix Chinese supply kit text
</commit_message>
<xml_diff>
--- a/translations/admin-strings-all.xlsx
+++ b/translations/admin-strings-all.xlsx
@@ -2673,9 +2673,6 @@
     <t>It's likely you have most items you need for your &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/FamilyDisasterSuppliesKitRedCross.pdf" target=_blank&gt;family supply kit&lt;/a&gt; already. Find out what else to add and get it organized before the next event hits. It's also a good idea to have an emergency &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/carkit.pdf" target=_blank&gt;car kit&lt;/a&gt;.</t>
   </si>
   <si>
-    <t>家庭用品套装中可能已经有您需要的大部分物品。 &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/FamilyDisasterSuppliesKitRedCross.pdf" &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/carkit.pdf" target=_blank&gt;汽车装备&lt;/a&gt;。target=_blank&gt;&lt;/a&gt;。了解如何在下一次事件到来之前补充并整理。最好能有一套应急的</t>
-  </si>
-  <si>
     <t>What to Expect at This Location</t>
   </si>
   <si>
@@ -3589,6 +3586,9 @@
   </si>
   <si>
     <t>Có vẻ như bạn đã có hầu hết các vật dụng cần thiết cho &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/FamilyDisasterSuppliesKitRedCross.pdf" target=_blank&gt;bộ dụng cụ khẩn cấp cho gia đình&lt;/a&gt; rồi. Tìm hiểu về các vật dụng nào cần bổ sung và sắp xếp vật dụng đó trước khi sự cố tiếp theo xảy ra. Một ý tưởng cũng rất hữu ích là có sẵn một &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/carkit.pdf" target=_blank&gt;bộ dụng cụ khẩn cấp trên xe&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>家庭用品套装中可能已经有您需要的大部分物品。 &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/FamilyDisasterSuppliesKitRedCross.pdf" target=_blank&gt;&lt;/a&gt;。了解如何在下一次事件到来之前补充并整理。最好能有一套应急的 &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/carkit.pdf" target=_blank&gt;汽车装备&lt;/a&gt;。</t>
   </si>
 </sst>
 </file>
@@ -4035,7 +4035,7 @@
   <dimension ref="A1:F96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4076,7 +4076,7 @@
         <v>172</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -4096,7 +4096,7 @@
         <v>173</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -4116,7 +4116,7 @@
         <v>174</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -4136,7 +4136,7 @@
         <v>175</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>9</v>
@@ -4156,7 +4156,7 @@
         <v>176</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -4176,7 +4176,7 @@
         <v>177</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
@@ -4196,7 +4196,7 @@
         <v>178</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
@@ -4216,7 +4216,7 @@
         <v>179</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>17</v>
@@ -4236,7 +4236,7 @@
         <v>180</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>19</v>
@@ -4256,7 +4256,7 @@
         <v>181</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
@@ -4276,7 +4276,7 @@
         <v>182</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>23</v>
@@ -4296,7 +4296,7 @@
         <v>183</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>25</v>
@@ -4316,7 +4316,7 @@
         <v>184</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>27</v>
@@ -4336,7 +4336,7 @@
         <v>185</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>29</v>
@@ -4376,7 +4376,7 @@
         <v>187</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>33</v>
@@ -4396,7 +4396,7 @@
         <v>188</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>35</v>
@@ -4410,22 +4410,22 @@
     </row>
     <row r="19" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>526</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="C19" s="16" t="s">
         <v>527</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="D19" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="6" t="s">
         <v>529</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="F19" s="19" t="s">
         <v>530</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="64" x14ac:dyDescent="0.25">
@@ -4436,7 +4436,7 @@
         <v>189</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>37</v>
@@ -4450,22 +4450,22 @@
     </row>
     <row r="21" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
+        <v>531</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>532</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="C21" s="16" t="s">
         <v>533</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="D21" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="6" t="s">
         <v>535</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="F21" s="19" t="s">
         <v>536</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="48" x14ac:dyDescent="0.25">
@@ -4476,7 +4476,7 @@
         <v>190</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>39</v>
@@ -4490,22 +4490,22 @@
     </row>
     <row r="23" spans="1:6" ht="256" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
+        <v>537</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>538</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="C23" s="16" t="s">
         <v>539</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="D23" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="6" t="s">
         <v>541</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="F23" s="19" t="s">
         <v>542</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="128" x14ac:dyDescent="0.25">
@@ -4516,7 +4516,7 @@
         <v>191</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>41</v>
@@ -4530,22 +4530,22 @@
     </row>
     <row r="25" spans="1:6" ht="368" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
+        <v>543</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>544</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="C25" s="16" t="s">
         <v>545</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="D25" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="6" t="s">
         <v>547</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="F25" s="19" t="s">
         <v>548</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="33" x14ac:dyDescent="0.25">
@@ -4556,7 +4556,7 @@
         <v>192</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>43</v>
@@ -4576,7 +4576,7 @@
         <v>193</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>45</v>
@@ -4596,7 +4596,7 @@
         <v>194</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>47</v>
@@ -4616,7 +4616,7 @@
         <v>195</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>49</v>
@@ -4636,7 +4636,7 @@
         <v>196</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>51</v>
@@ -4656,7 +4656,7 @@
         <v>197</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>53</v>
@@ -4676,7 +4676,7 @@
         <v>198</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>55</v>
@@ -4696,7 +4696,7 @@
         <v>199</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>57</v>
@@ -4716,7 +4716,7 @@
         <v>200</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>59</v>
@@ -4736,7 +4736,7 @@
         <v>201</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>61</v>
@@ -4756,7 +4756,7 @@
         <v>202</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>63</v>
@@ -4776,7 +4776,7 @@
         <v>203</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>65</v>
@@ -4796,7 +4796,7 @@
         <v>204</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>67</v>
@@ -4816,7 +4816,7 @@
         <v>205</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>69</v>
@@ -4876,7 +4876,7 @@
         <v>208</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>75</v>
@@ -4896,7 +4896,7 @@
         <v>209</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>77</v>
@@ -4916,7 +4916,7 @@
         <v>210</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>79</v>
@@ -4936,7 +4936,7 @@
         <v>211</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>81</v>
@@ -4956,7 +4956,7 @@
         <v>212</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>83</v>
@@ -4976,7 +4976,7 @@
         <v>213</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>85</v>
@@ -4996,7 +4996,7 @@
         <v>214</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>87</v>
@@ -5016,7 +5016,7 @@
         <v>215</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>89</v>
@@ -5036,7 +5036,7 @@
         <v>216</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>91</v>
@@ -5056,7 +5056,7 @@
         <v>217</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>93</v>
@@ -5076,7 +5076,7 @@
         <v>218</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>95</v>
@@ -5096,7 +5096,7 @@
         <v>219</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>97</v>
@@ -5116,7 +5116,7 @@
         <v>220</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>99</v>
@@ -5136,7 +5136,7 @@
         <v>221</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>101</v>
@@ -5156,7 +5156,7 @@
         <v>222</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>103</v>
@@ -5176,7 +5176,7 @@
         <v>223</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>105</v>
@@ -5196,7 +5196,7 @@
         <v>224</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>107</v>
@@ -5236,7 +5236,7 @@
         <v>226</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>111</v>
@@ -5256,7 +5256,7 @@
         <v>227</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>113</v>
@@ -5276,7 +5276,7 @@
         <v>228</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>115</v>
@@ -5296,7 +5296,7 @@
         <v>229</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>117</v>
@@ -5316,7 +5316,7 @@
         <v>230</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>119</v>
@@ -5336,7 +5336,7 @@
         <v>231</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>121</v>
@@ -5356,7 +5356,7 @@
         <v>232</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>123</v>
@@ -5376,7 +5376,7 @@
         <v>233</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>125</v>
@@ -5396,7 +5396,7 @@
         <v>234</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>127</v>
@@ -5416,7 +5416,7 @@
         <v>235</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>129</v>
@@ -5436,7 +5436,7 @@
         <v>236</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>131</v>
@@ -5456,7 +5456,7 @@
         <v>237</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>133</v>
@@ -5476,7 +5476,7 @@
         <v>238</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>135</v>
@@ -5496,7 +5496,7 @@
         <v>239</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>137</v>
@@ -5516,7 +5516,7 @@
         <v>240</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>139</v>
@@ -5536,7 +5536,7 @@
         <v>241</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>141</v>
@@ -5556,7 +5556,7 @@
         <v>242</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>143</v>
@@ -5576,7 +5576,7 @@
         <v>243</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>145</v>
@@ -5596,7 +5596,7 @@
         <v>244</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>147</v>
@@ -5616,7 +5616,7 @@
         <v>245</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>149</v>
@@ -5636,7 +5636,7 @@
         <v>246</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>151</v>
@@ -5656,7 +5656,7 @@
         <v>247</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>153</v>
@@ -5676,7 +5676,7 @@
         <v>248</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>155</v>
@@ -5696,7 +5696,7 @@
         <v>249</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>157</v>
@@ -5716,7 +5716,7 @@
         <v>250</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>159</v>
@@ -5736,7 +5736,7 @@
         <v>251</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>161</v>
@@ -5776,10 +5776,10 @@
         <v>253</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>345</v>
@@ -5796,7 +5796,7 @@
         <v>254</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>166</v>
@@ -5816,7 +5816,7 @@
         <v>255</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>168</v>
@@ -5836,7 +5836,7 @@
         <v>256</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>170</v>
@@ -5853,39 +5853,39 @@
         <v>435</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>436</v>
+        <v>551</v>
       </c>
       <c r="C91" s="16" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E91" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="F91" s="19" t="s">
         <v>550</v>
-      </c>
-      <c r="F91" s="19" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
+        <v>436</v>
+      </c>
+      <c r="B92" s="12" t="s">
         <v>437</v>
       </c>
-      <c r="B92" s="12" t="s">
-        <v>438</v>
-      </c>
       <c r="C92" s="13" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D92" s="13" t="s">
+        <v>522</v>
+      </c>
+      <c r="E92" s="13" t="s">
         <v>523</v>
       </c>
-      <c r="E92" s="13" t="s">
+      <c r="F92" s="11" t="s">
         <v>524</v>
-      </c>
-      <c r="F92" s="11" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Chinese 'about' text had weird markup
</commit_message>
<xml_diff>
--- a/translations/admin-strings-all.xlsx
+++ b/translations/admin-strings-all.xlsx
@@ -1452,9 +1452,6 @@
     <t>您所在地区随时可能自然灾害。了解您在华盛顿州金县的那个地方生活、工作或娱乐。</t>
   </si>
   <si>
-    <t>这是以 &lt;a href="http://www.opb.org/news/widget/aftershock-find-your-cascadia-earthquake-story/" target="_blank"&gt;Aftershock&lt;/a&gt;面向俄勒冈居民的地震准备申请为基础的。&lt;a href="https://www.linkedin.com/in/carson-macpherson-krutsky-400645105" target="_blank"&gt;Carson MacPherson-Krutsky&lt;/a&gt; 和 &lt;a href="https://hs.umt.edu/geosciences/faculty/bendick/" target="_blank"&gt; Rebecca Bendick 博士&lt;/a&gt;——蒙大拿大学的一名研究生及其导师——意欲扩大范围至其他当地人，并增加灾害类型。&lt;a href="https://github.com/nein09" target="_blank"&gt;Melinda Minch&lt;/a&gt; 和 &lt;a href="https://github.com/eldang" target="_blank"&gt;Eldan Goldenberg&lt;/a&gt; 为该目的采用了该想法。本网站的通用版本来源可从 &lt;a href="https://github.com/missoula-ready/disaster-preparedness" target="_blank"&gt;Github&lt;/a&gt; 上获取。&lt;br/&gt; 几家实体支持的内容和数据，包括蒙大拿大学和西雅图市。 &lt;a href="http://www.umt.edu/" alt="logo" target="_blank"&gt;&lt;/a&gt;, &lt;a href="http://www.kingcounty.gov/" alt="logo" target="_blank"&gt;King County&lt;/a&gt;, and the &lt;a href="http://www.seattle.gov/" alt="logo" target="_blank"&gt;&lt;/a&gt;。</t>
-  </si>
-  <si>
     <t>近期历史</t>
   </si>
   <si>
@@ -3589,6 +3586,9 @@
   </si>
   <si>
     <t>家庭用品套装中可能已经有您需要的大部分物品。 &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/FamilyDisasterSuppliesKitRedCross.pdf" target=_blank&gt;&lt;/a&gt;。了解如何在下一次事件到来之前补充并整理。最好能有一套应急的 &lt;a href="http://www.seattle.gov/Documents/Departments/Emergency/Preparedness/FamilyPlans/carkit.pdf" target=_blank&gt;汽车装备&lt;/a&gt;。</t>
+  </si>
+  <si>
+    <t>这是以 &lt;a href="http://www.opb.org/news/widget/aftershock-find-your-cascadia-earthquake-story/" target="_blank"&gt;Aftershock&lt;/a&gt;面向俄勒冈居民的地震准备申请为基础的。&lt;a href="https://www.linkedin.com/in/carson-macpherson-krutsky-400645105" target="_blank"&gt;Carson MacPherson-Krutsky&lt;/a&gt; 和 &lt;a href="https://hs.umt.edu/geosciences/faculty/bendick/" target="_blank"&gt; Rebecca Bendick 博士&lt;/a&gt;——蒙大拿大学的一名研究生及其导师——意欲扩大范围至其他当地人，并增加灾害类型。&lt;a href="https://github.com/nein09" target="_blank"&gt;Melinda Minch&lt;/a&gt; 和 &lt;a href="https://github.com/eldang" target="_blank"&gt;Eldan Goldenberg&lt;/a&gt; 为该目的采用了该想法。本网站的通用版本来源可从 &lt;a href="https://github.com/missoula-ready/disaster-preparedness" target="_blank"&gt;Github&lt;/a&gt; 上获取。&lt;br/&gt; 几家实体支持的内容和数据，包括蒙大拿大学和西雅图市。 &lt;a href="http://www.umt.edu/" alt="logo" target="_blank"&gt;蒙大拿大学&lt;/a&gt;, &lt;a href="http://www.kingcounty.gov/" alt="logo" target="_blank"&gt;金县&lt;/a&gt;，&lt;a href="http://www.seattle.gov/" alt="logo" target="_blank"&gt;与西雅图市的共同合作&lt;/a&gt;。</t>
   </si>
 </sst>
 </file>
@@ -4034,8 +4034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4056,16 +4056,16 @@
         <v>171</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="81" x14ac:dyDescent="0.25">
@@ -4076,16 +4076,16 @@
         <v>172</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="65" x14ac:dyDescent="0.25">
@@ -4096,16 +4096,16 @@
         <v>173</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="97" x14ac:dyDescent="0.25">
@@ -4116,16 +4116,16 @@
         <v>174</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="49" x14ac:dyDescent="0.25">
@@ -4136,16 +4136,16 @@
         <v>175</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.25">
@@ -4156,16 +4156,16 @@
         <v>176</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="81" x14ac:dyDescent="0.25">
@@ -4176,16 +4176,16 @@
         <v>177</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="65" x14ac:dyDescent="0.25">
@@ -4196,16 +4196,16 @@
         <v>178</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="80" x14ac:dyDescent="0.25">
@@ -4216,16 +4216,16 @@
         <v>179</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="65" x14ac:dyDescent="0.25">
@@ -4236,16 +4236,16 @@
         <v>180</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="65" x14ac:dyDescent="0.25">
@@ -4256,16 +4256,16 @@
         <v>181</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="112" x14ac:dyDescent="0.25">
@@ -4276,16 +4276,16 @@
         <v>182</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="49" x14ac:dyDescent="0.25">
@@ -4296,16 +4296,16 @@
         <v>183</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="64" x14ac:dyDescent="0.25">
@@ -4316,16 +4316,16 @@
         <v>184</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.25">
@@ -4336,16 +4336,16 @@
         <v>185</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="80" x14ac:dyDescent="0.25">
@@ -4356,16 +4356,16 @@
         <v>186</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="81" x14ac:dyDescent="0.25">
@@ -4376,16 +4376,16 @@
         <v>187</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="112" x14ac:dyDescent="0.25">
@@ -4396,36 +4396,36 @@
         <v>188</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>524</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>525</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="C19" s="16" t="s">
         <v>526</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="D19" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="F19" s="19" t="s">
         <v>529</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="64" x14ac:dyDescent="0.25">
@@ -4436,36 +4436,36 @@
         <v>189</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
+        <v>530</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>531</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="C21" s="16" t="s">
         <v>532</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="D21" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="F21" s="19" t="s">
         <v>535</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="48" x14ac:dyDescent="0.25">
@@ -4476,36 +4476,36 @@
         <v>190</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="256" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
+        <v>536</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>537</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="C23" s="16" t="s">
         <v>538</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="D23" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="6" t="s">
         <v>540</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="F23" s="19" t="s">
         <v>541</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="128" x14ac:dyDescent="0.25">
@@ -4516,36 +4516,36 @@
         <v>191</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="368" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>543</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="C25" s="16" t="s">
         <v>544</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="D25" s="3" t="s">
         <v>545</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="6" t="s">
         <v>546</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="F25" s="19" t="s">
         <v>547</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="33" x14ac:dyDescent="0.25">
@@ -4556,16 +4556,16 @@
         <v>192</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="320" x14ac:dyDescent="0.25">
@@ -4576,16 +4576,16 @@
         <v>193</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="368" x14ac:dyDescent="0.25">
@@ -4596,16 +4596,16 @@
         <v>194</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4616,16 +4616,16 @@
         <v>195</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4636,16 +4636,16 @@
         <v>196</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="409" x14ac:dyDescent="0.25">
@@ -4656,16 +4656,16 @@
         <v>197</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4676,16 +4676,16 @@
         <v>198</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>55</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4696,16 +4696,16 @@
         <v>199</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>57</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="304" x14ac:dyDescent="0.25">
@@ -4716,16 +4716,16 @@
         <v>200</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="368" x14ac:dyDescent="0.25">
@@ -4736,16 +4736,16 @@
         <v>201</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>61</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4756,16 +4756,16 @@
         <v>202</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>63</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4776,16 +4776,16 @@
         <v>203</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4796,16 +4796,16 @@
         <v>204</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>67</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="192" x14ac:dyDescent="0.25">
@@ -4816,16 +4816,16 @@
         <v>205</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>69</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="384" x14ac:dyDescent="0.25">
@@ -4836,16 +4836,16 @@
         <v>206</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="224" x14ac:dyDescent="0.25">
@@ -4856,16 +4856,16 @@
         <v>207</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="409" x14ac:dyDescent="0.25">
@@ -4876,16 +4876,16 @@
         <v>208</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>75</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="176" x14ac:dyDescent="0.25">
@@ -4896,16 +4896,16 @@
         <v>209</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>77</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="400" x14ac:dyDescent="0.25">
@@ -4916,16 +4916,16 @@
         <v>210</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4936,16 +4936,16 @@
         <v>211</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="304" x14ac:dyDescent="0.25">
@@ -4956,16 +4956,16 @@
         <v>212</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4976,16 +4976,16 @@
         <v>213</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F47" s="17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4996,16 +4996,16 @@
         <v>214</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -5016,16 +5016,16 @@
         <v>215</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="409" x14ac:dyDescent="0.25">
@@ -5036,16 +5036,16 @@
         <v>216</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="304" x14ac:dyDescent="0.25">
@@ -5056,16 +5056,16 @@
         <v>217</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>93</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F51" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="400" x14ac:dyDescent="0.25">
@@ -5076,16 +5076,16 @@
         <v>218</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>95</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F52" s="17" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -5096,16 +5096,16 @@
         <v>219</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>97</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -5116,16 +5116,16 @@
         <v>220</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>99</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -5136,16 +5136,16 @@
         <v>221</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>101</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -5156,16 +5156,16 @@
         <v>222</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>103</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -5176,16 +5176,16 @@
         <v>223</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="409" x14ac:dyDescent="0.25">
@@ -5196,16 +5196,16 @@
         <v>224</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>107</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -5216,16 +5216,16 @@
         <v>225</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F59" s="17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -5236,16 +5236,16 @@
         <v>226</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>111</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F60" s="17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="400" x14ac:dyDescent="0.25">
@@ -5256,16 +5256,16 @@
         <v>227</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>113</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F61" s="17" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="409" x14ac:dyDescent="0.25">
@@ -5276,16 +5276,16 @@
         <v>228</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>115</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="352" x14ac:dyDescent="0.25">
@@ -5296,16 +5296,16 @@
         <v>229</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="409" x14ac:dyDescent="0.25">
@@ -5316,16 +5316,16 @@
         <v>230</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>119</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="409" x14ac:dyDescent="0.25">
@@ -5336,16 +5336,16 @@
         <v>231</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>121</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="409" x14ac:dyDescent="0.25">
@@ -5356,16 +5356,16 @@
         <v>232</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>123</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -5376,16 +5376,16 @@
         <v>233</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>125</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F67" s="17" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="409" x14ac:dyDescent="0.25">
@@ -5396,16 +5396,16 @@
         <v>234</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>127</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F68" s="17" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -5416,16 +5416,16 @@
         <v>235</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>129</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -5436,16 +5436,16 @@
         <v>236</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>131</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="409" x14ac:dyDescent="0.25">
@@ -5456,16 +5456,16 @@
         <v>237</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -5476,16 +5476,16 @@
         <v>238</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="409" x14ac:dyDescent="0.25">
@@ -5496,16 +5496,16 @@
         <v>239</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>137</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="400" x14ac:dyDescent="0.25">
@@ -5516,16 +5516,16 @@
         <v>240</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>139</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="33" x14ac:dyDescent="0.25">
@@ -5536,16 +5536,16 @@
         <v>241</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="48" x14ac:dyDescent="0.25">
@@ -5556,16 +5556,16 @@
         <v>242</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>143</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="33" x14ac:dyDescent="0.25">
@@ -5576,16 +5576,16 @@
         <v>243</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>145</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F77" s="17" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="33" x14ac:dyDescent="0.25">
@@ -5596,16 +5596,16 @@
         <v>244</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>147</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F78" s="17" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="33" x14ac:dyDescent="0.25">
@@ -5616,16 +5616,16 @@
         <v>245</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>149</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F79" s="17" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="32" x14ac:dyDescent="0.25">
@@ -5636,16 +5636,16 @@
         <v>246</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>151</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F80" s="17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="33" x14ac:dyDescent="0.25">
@@ -5656,16 +5656,16 @@
         <v>247</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>153</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="368" x14ac:dyDescent="0.25">
@@ -5676,16 +5676,16 @@
         <v>248</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>155</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="192" x14ac:dyDescent="0.25">
@@ -5696,16 +5696,16 @@
         <v>249</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>157</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="65" x14ac:dyDescent="0.25">
@@ -5716,16 +5716,16 @@
         <v>250</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>159</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F84" s="17" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="112" x14ac:dyDescent="0.25">
@@ -5736,16 +5736,16 @@
         <v>251</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>161</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F85" s="17" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="336" x14ac:dyDescent="0.25">
@@ -5756,16 +5756,16 @@
         <v>252</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>163</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F86" s="17" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -5773,19 +5773,19 @@
         <v>164</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>253</v>
+        <v>551</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F87" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="48" x14ac:dyDescent="0.25">
@@ -5793,19 +5793,19 @@
         <v>165</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>166</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F88" s="17" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="49" x14ac:dyDescent="0.25">
@@ -5813,19 +5813,19 @@
         <v>167</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>168</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F89" s="17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="33" x14ac:dyDescent="0.25">
@@ -5833,59 +5833,59 @@
         <v>169</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>170</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F90" s="17" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C91" s="16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E91" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="F91" s="19" t="s">
         <v>549</v>
-      </c>
-      <c r="F91" s="19" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
+        <v>435</v>
+      </c>
+      <c r="B92" s="12" t="s">
         <v>436</v>
       </c>
-      <c r="B92" s="12" t="s">
-        <v>437</v>
-      </c>
       <c r="C92" s="13" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D92" s="13" t="s">
+        <v>521</v>
+      </c>
+      <c r="E92" s="13" t="s">
         <v>522</v>
       </c>
-      <c r="E92" s="13" t="s">
+      <c r="F92" s="11" t="s">
         <v>523</v>
-      </c>
-      <c r="F92" s="11" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix things like missing parentheses and typos in English
</commit_message>
<xml_diff>
--- a/translations/admin-strings-all.xlsx
+++ b/translations/admin-strings-all.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="2180" windowWidth="27360" windowHeight="15880" tabRatio="500"/>
+    <workbookView xWindow="3960" yWindow="780" windowWidth="27360" windowHeight="15880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -601,9 +601,6 @@
     </r>
   </si>
   <si>
-    <t>In December 1921, torrential rains caused train wrecks, washed out bridges, and flooded Seattle streets and neighborhoods.Three people  were burried under this slide in West Seattle when their house was swept away by a landslide. (credit: MOHAI, PEMCO Webster &amp; Stevens Collection)</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -797,20 +794,6 @@
     </r>
   </si>
   <si>
-    <t>After the earthquake destroyed the outside wall of their architecture office in Pioneer Square, a couple finish removing items from the debris. (Tom Reese/The Seattle Times</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Dhul gariirka kadib dhulgariirka wuxuu baabi’iyay banaanka darbiga ee xafiiskooda naqshada ee Pioneer Square, lamaanaha dhameeyo ka saarida sheeyada haraaga. (Tom Reese/The Seattle Times</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">The Nisqually earthquake on Feb. 28, 2001, caused damage in Pioneer Square, including to this vehicle on Second Avenue and South Jackson that was showered with bricks. (Greg Gilbert/The Seattle Times) </t>
   </si>
   <si>
@@ -1374,9 +1357,6 @@
     <t>这张照片是伦顿附近被淹没的奥里利亚镇的空中俯瞰图。1933 年 12 月中旬，一个多星期的大雨导致华盛顿州西部多发泥石流和洪水。12 月 10 日，《西雅图时报》报道所有地区的河流都逼近洪水位。杜瓦米河、绿河和白河水位超过河岸，流向河谷中的城镇。（致谢：MOHAI，PEMCO Webster ＆ Stevens Collection）</t>
   </si>
   <si>
-    <t>地震摧毁了先锋广场上的建筑事务所的外墙后，一对夫妇停止从碎片中搬出物品。(Tom Reese/The Seattle Times</t>
-  </si>
-  <si>
     <t xml:space="preserve">2001 年 2 月 28 日的尼斯凯里地震在先锋广场造成了破坏，包括第 2 大道和 South Jackson 被砖头砸坏的这辆车。(Greg Gilbert/The Seattle Times) </t>
   </si>
   <si>
@@ -2094,17 +2074,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Una pareja terminando de recuperar elementos entre los escombros luego de que el terremoto haya destruido la pared externa de su oficina de arquitectura en Pioneer Square. (Tom Reese / The Seattle Times</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve">El terremoto de Nisqually del 28 de febrero de 2001, causó daños en Pioneer Square, incluido este vehículo en Second Avenue y South Jackson que estaba cubierto de ladrillos. (Greg Gilbert / The Seattle Times) </t>
     </r>
   </si>
@@ -2577,9 +2546,6 @@
     <t>Bức ảnh này chụp từ trên cao cảnh thị trấn Orillia, gần Renton bị ngập lụt. Trong hơn một tuần mưa to kéo dài vào giữa tháng Mười Hai năm 1933 gây ra lở đất và lũ lụt khắp miền tây tiểu bang Washington. Vào ngày 10 tháng Mười Hai, tờ Seattle Times đưa tin tất cả các sông trong trung vực đã gần mức tràn nước. Sông Duwamish, Green và White đã tràn qua bờ, gây lũ lụt cho các thị trấn dọc thung lũng. (ảnh thuộc về: MOHAI, Bộ sưu tập PEMCO Webster &amp; Stevens)</t>
   </si>
   <si>
-    <t>Sau khi trận động đất phá huỷ bức tường bên ngoài văn phòng kiến trúc của họ tại Quảng Trường Pioneer, một cặp đôi đã dừng di dời đồ vật từ đống đổ nát. (Tom Reese/The Seattle Times</t>
-  </si>
-  <si>
     <t xml:space="preserve">Trận động đất Nisqually xảy ra vào ngày 28 tháng Hai năm 2001, đã gây thiệt hại cho Quảng Trường Pioneer, trong đó bao gồm hình ảnh đống gạch vụn trút xuống phương tiện này trên đại lộ Second Avenue và South Jackson. (Greg Gilbert/The Seattle Times) </t>
   </si>
   <si>
@@ -3589,6 +3555,24 @@
   </si>
   <si>
     <t>这是以 &lt;a href="http://www.opb.org/news/widget/aftershock-find-your-cascadia-earthquake-story/" target="_blank"&gt;Aftershock&lt;/a&gt;面向俄勒冈居民的地震准备申请为基础的。&lt;a href="https://www.linkedin.com/in/carson-macpherson-krutsky-400645105" target="_blank"&gt;Carson MacPherson-Krutsky&lt;/a&gt; 和 &lt;a href="https://hs.umt.edu/geosciences/faculty/bendick/" target="_blank"&gt; Rebecca Bendick 博士&lt;/a&gt;——蒙大拿大学的一名研究生及其导师——意欲扩大范围至其他当地人，并增加灾害类型。&lt;a href="https://github.com/nein09" target="_blank"&gt;Melinda Minch&lt;/a&gt; 和 &lt;a href="https://github.com/eldang" target="_blank"&gt;Eldan Goldenberg&lt;/a&gt; 为该目的采用了该想法。本网站的通用版本来源可从 &lt;a href="https://github.com/missoula-ready/disaster-preparedness" target="_blank"&gt;Github&lt;/a&gt; 上获取。&lt;br/&gt; 几家实体支持的内容和数据，包括蒙大拿大学和西雅图市。 &lt;a href="http://www.umt.edu/" alt="logo" target="_blank"&gt;蒙大拿大学&lt;/a&gt;, &lt;a href="http://www.kingcounty.gov/" alt="logo" target="_blank"&gt;金县&lt;/a&gt;，&lt;a href="http://www.seattle.gov/" alt="logo" target="_blank"&gt;与西雅图市的共同合作&lt;/a&gt;。</t>
+  </si>
+  <si>
+    <t>After the earthquake destroyed the outside wall of their architecture office in Pioneer Square, a couple finish removing items from the debris. (Tom Reese/The Seattle Times)</t>
+  </si>
+  <si>
+    <t>地震摧毁了先锋广场上的建筑事务所的外墙后，一对夫妇停止从碎片中搬出物品。(Tom Reese/The Seattle Times)</t>
+  </si>
+  <si>
+    <t>Dhul gariirka kadib dhulgariirka wuxuu baabi’iyay banaanka darbiga ee xafiiskooda naqshada ee Pioneer Square, lamaanaha dhameeyo ka saarida sheeyada haraaga. (Tom Reese/The Seattle Times)</t>
+  </si>
+  <si>
+    <t>Una pareja terminando de recuperar elementos entre los escombros luego de que el terremoto haya destruido la pared externa de su oficina de arquitectura en Pioneer Square. (Tom Reese / The Seattle Times)</t>
+  </si>
+  <si>
+    <t>Sau khi trận động đất phá huỷ bức tường bên ngoài văn phòng kiến trúc của họ tại Quảng Trường Pioneer, một cặp đôi đã dừng di dời đồ vật từ đống đổ nát. (Tom Reese/The Seattle Times)</t>
+  </si>
+  <si>
+    <t>In December 1921, torrential rains caused train wrecks, washed out bridges, and flooded Seattle streets and neighborhoods.Three people  were buried under this slide in West Seattle when their house was swept away by a landslide. (credit: MOHAI, PEMCO Webster &amp; Stevens Collection)</t>
   </si>
 </sst>
 </file>
@@ -4034,8 +4018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4053,19 +4037,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="81" x14ac:dyDescent="0.25">
@@ -4073,19 +4057,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="65" x14ac:dyDescent="0.25">
@@ -4093,19 +4077,19 @@
         <v>4</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="97" x14ac:dyDescent="0.25">
@@ -4113,19 +4097,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="49" x14ac:dyDescent="0.25">
@@ -4133,19 +4117,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.25">
@@ -4153,19 +4137,19 @@
         <v>10</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="81" x14ac:dyDescent="0.25">
@@ -4173,19 +4157,19 @@
         <v>12</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="65" x14ac:dyDescent="0.25">
@@ -4193,19 +4177,19 @@
         <v>14</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="80" x14ac:dyDescent="0.25">
@@ -4213,19 +4197,19 @@
         <v>16</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="65" x14ac:dyDescent="0.25">
@@ -4233,19 +4217,19 @@
         <v>18</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="65" x14ac:dyDescent="0.25">
@@ -4253,19 +4237,19 @@
         <v>20</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="112" x14ac:dyDescent="0.25">
@@ -4273,19 +4257,19 @@
         <v>22</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="49" x14ac:dyDescent="0.25">
@@ -4293,19 +4277,19 @@
         <v>24</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="64" x14ac:dyDescent="0.25">
@@ -4313,19 +4297,19 @@
         <v>26</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.25">
@@ -4333,19 +4317,19 @@
         <v>28</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="80" x14ac:dyDescent="0.25">
@@ -4353,19 +4337,19 @@
         <v>30</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="81" x14ac:dyDescent="0.25">
@@ -4373,19 +4357,19 @@
         <v>32</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="112" x14ac:dyDescent="0.25">
@@ -4393,39 +4377,39 @@
         <v>34</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="64" x14ac:dyDescent="0.25">
@@ -4433,39 +4417,39 @@
         <v>36</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="48" x14ac:dyDescent="0.25">
@@ -4473,39 +4457,39 @@
         <v>38</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="256" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="128" x14ac:dyDescent="0.25">
@@ -4513,39 +4497,39 @@
         <v>40</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="368" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="33" x14ac:dyDescent="0.25">
@@ -4553,19 +4537,19 @@
         <v>42</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="320" x14ac:dyDescent="0.25">
@@ -4573,19 +4557,19 @@
         <v>44</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="368" x14ac:dyDescent="0.25">
@@ -4593,19 +4577,19 @@
         <v>46</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4613,19 +4597,19 @@
         <v>48</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4633,19 +4617,19 @@
         <v>50</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="409" x14ac:dyDescent="0.25">
@@ -4653,19 +4637,19 @@
         <v>52</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4673,19 +4657,19 @@
         <v>54</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>55</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4693,19 +4677,19 @@
         <v>56</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>57</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="304" x14ac:dyDescent="0.25">
@@ -4713,19 +4697,19 @@
         <v>58</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="368" x14ac:dyDescent="0.25">
@@ -4733,19 +4717,19 @@
         <v>60</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>61</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4753,19 +4737,19 @@
         <v>62</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>63</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4773,19 +4757,19 @@
         <v>64</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4793,19 +4777,19 @@
         <v>66</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>67</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="192" x14ac:dyDescent="0.25">
@@ -4813,19 +4797,19 @@
         <v>68</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>69</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="384" x14ac:dyDescent="0.25">
@@ -4833,19 +4817,19 @@
         <v>70</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="224" x14ac:dyDescent="0.25">
@@ -4853,19 +4837,19 @@
         <v>72</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="409" x14ac:dyDescent="0.25">
@@ -4873,19 +4857,19 @@
         <v>74</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>75</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="176" x14ac:dyDescent="0.25">
@@ -4893,19 +4877,19 @@
         <v>76</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>77</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="400" x14ac:dyDescent="0.25">
@@ -4913,19 +4897,19 @@
         <v>78</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
@@ -4933,19 +4917,19 @@
         <v>80</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="304" x14ac:dyDescent="0.25">
@@ -4953,939 +4937,939 @@
         <v>82</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>475</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="E47" s="5" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F47" s="17" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>470</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>476</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="E48" s="5" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>471</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>477</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="E49" s="5" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>472</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B50" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>478</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="E50" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="304" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>473</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B51" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>479</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="E51" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F51" s="17" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="400" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>474</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B52" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>480</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="E52" s="5" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F52" s="17" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>475</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>481</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="E53" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>476</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>482</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="E54" s="5" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>477</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B55" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>483</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="E55" s="5" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>478</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B56" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>484</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="E56" s="5" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>479</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B57" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="C57" s="15" t="s">
-        <v>485</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="E57" s="5" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>480</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B58" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="C58" s="15" t="s">
-        <v>486</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="E58" s="5" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B59" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="E59" s="5" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="F59" s="17" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>481</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B60" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>487</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="E60" s="5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F60" s="17" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="400" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>112</v>
+        <v>546</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>227</v>
+        <v>547</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>488</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="F61" s="17" t="s">
-        <v>404</v>
+        <v>482</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="352" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="F67" s="17" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F68" s="17" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="409" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="400" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="48" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F77" s="17" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F78" s="17" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="F79" s="17" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="32" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F80" s="17" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="368" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="192" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="65" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="F84" s="17" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="112" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="F85" s="17" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="336" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="F86" s="17" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="C87" s="15" t="s">
+        <v>507</v>
+      </c>
+      <c r="D87" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="D87" s="3" t="s">
-        <v>519</v>
-      </c>
       <c r="E87" s="6" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F87" s="17" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="48" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F88" s="17" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="49" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="F89" s="17" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="F90" s="17" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="C91" s="16" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="F91" s="19" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="D92" s="13" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="F92" s="11" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add final text, pad snuggets a little
</commit_message>
<xml_diff>
--- a/translations/admin-strings-all.xlsx
+++ b/translations/admin-strings-all.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="780" windowWidth="27360" windowHeight="15880" tabRatio="500"/>
+    <workbookView xWindow="3120" yWindow="460" windowWidth="27360" windowHeight="15880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="642">
   <si>
     <t>English</t>
   </si>
@@ -176,17 +176,6 @@
   </si>
   <si>
     <t>Earthquake: Unreinforced Masonry Buildings</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Dhulgariirka: Dhismooyinka Bulkeetiga Culus</t>
-    </r>
   </si>
   <si>
     <t>Earthquake: Tsunami</t>
@@ -3729,6 +3718,135 @@
   </si>
   <si>
     <t>Nếu đập bị vỡ</t>
+  </si>
+  <si>
+    <t>Climate Impacts</t>
+  </si>
+  <si>
+    <t>Impactos climáticos</t>
+  </si>
+  <si>
+    <t>Saamaynta Cimilada</t>
+  </si>
+  <si>
+    <t>Влияние климата</t>
+  </si>
+  <si>
+    <t>Tác động của Khí hậu</t>
+  </si>
+  <si>
+    <t>气候影响</t>
+  </si>
+  <si>
+    <t>侵蚀风险</t>
+  </si>
+  <si>
+    <t>Erosion Risk</t>
+  </si>
+  <si>
+    <t>риск возникновения эрозии</t>
+  </si>
+  <si>
+    <t>Halista Nabaadguurka</t>
+  </si>
+  <si>
+    <t>Riesgo de Erosión.</t>
+  </si>
+  <si>
+    <t>Nguy Cơ Xói Mòn</t>
+  </si>
+  <si>
+    <t>Local Resources</t>
+  </si>
+  <si>
+    <t>Khayraadka Deegaanka</t>
+  </si>
+  <si>
+    <t>本地资源</t>
+  </si>
+  <si>
+    <t>Местные ресурсы</t>
+  </si>
+  <si>
+    <t>Recursos locales</t>
+  </si>
+  <si>
+    <t>Tài nguyên Địa phương</t>
+  </si>
+  <si>
+    <t>Warning Signs</t>
+  </si>
+  <si>
+    <t>警告标志</t>
+  </si>
+  <si>
+    <t>Предупреждающие знаки</t>
+  </si>
+  <si>
+    <t>Calaamadaha Digniinta</t>
+  </si>
+  <si>
+    <t>Señales de advertencia</t>
+  </si>
+  <si>
+    <t>Dấu hiệu cảnh báo</t>
+  </si>
+  <si>
+    <t>Unstable Structures</t>
+  </si>
+  <si>
+    <t>Cấu trúc không ổn định</t>
+  </si>
+  <si>
+    <t>Estructuras Inestables</t>
+  </si>
+  <si>
+    <t>Dhismayaasha aan degganeyn</t>
+  </si>
+  <si>
+    <t>Нестабильные структуры</t>
+  </si>
+  <si>
+    <t>不稳定结构</t>
+  </si>
+  <si>
+    <t>Liquefaction</t>
+  </si>
+  <si>
+    <t>液化</t>
+  </si>
+  <si>
+    <t>разжижение грунтов</t>
+  </si>
+  <si>
+    <t>Godadka</t>
+  </si>
+  <si>
+    <t>Licuefacción</t>
+  </si>
+  <si>
+    <t>Hoá Lỏng Đất</t>
+  </si>
+  <si>
+    <t>In Your Lifetime</t>
+  </si>
+  <si>
+    <t>在你的终身</t>
+  </si>
+  <si>
+    <t>В вашей жизни</t>
+  </si>
+  <si>
+    <t>Waqtigaaga Lifaaqa</t>
+  </si>
+  <si>
+    <t>Trong suốt tuổi thọ</t>
+  </si>
+  <si>
+    <t>Dhulgariirka: Dhismooyinka Bulkeetiga Culus</t>
+  </si>
+  <si>
+    <t>En su vida</t>
   </si>
 </sst>
 </file>
@@ -3822,12 +3940,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -3858,7 +3982,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3915,6 +4039,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4193,2020 +4327,2160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="F93" sqref="F93:F100"/>
+    <sheetView tabSelected="1" topLeftCell="C91" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="75.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="61" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="9"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="10.83203125" style="5"/>
-    <col min="6" max="6" width="10.83203125" style="18"/>
+    <col min="2" max="2" width="61.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.6640625" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="81" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="65" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="97" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="49" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="81" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="65" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="80" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="65" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="65" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="112" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>439</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C13" s="15" t="s">
         <v>440</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="5" t="s">
+      <c r="D13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F13" s="17" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="49" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="10" t="s">
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C14" s="15" t="s">
         <v>441</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="D14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F14" s="17" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="64" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="10" t="s">
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C15" s="15" t="s">
         <v>442</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="D15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F15" s="17" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="10" t="s">
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C16" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>443</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="80" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="C16" s="16" t="s">
+      <c r="D17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>444</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="80" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>516</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>517</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>518</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>445</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="81" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>523</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>524</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="65" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>528</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>529</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>530</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>447</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>535</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>536</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>448</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="65" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="128" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>451</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="112" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>452</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>453</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="129" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="176" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>455</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="129" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>458</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="96" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>459</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="81" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>460</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>461</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C40" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="81" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>444</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="112" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>445</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="409" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>517</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>518</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>519</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>520</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>521</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="64" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>446</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="409" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>523</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>524</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>525</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>527</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>447</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="256" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>529</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>530</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>531</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>532</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>533</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="128" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>448</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="368" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>535</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>536</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>537</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>539</v>
-      </c>
-      <c r="F25" s="19" t="s">
+      <c r="D40" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="80" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>463</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="65" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="81" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>466</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="97" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>467</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="177" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>468</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="96" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="65" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>470</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="48" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>471</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>472</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="128" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>473</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="131" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>474</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="160" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>475</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="F55" s="17" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="129" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>476</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="F56" s="17" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="129" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>477</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="80" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>478</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="160" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="161" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>479</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="F60" s="17" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="65" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
+        <v>544</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>545</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>480</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="80" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>481</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="F62" s="17" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>482</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="80" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>483</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="F64" s="17" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="65" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>484</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="F65" s="17" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="81" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>485</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="F66" s="17" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="96" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>486</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="F67" s="17" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="96" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="F68" s="17" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="128" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="F69" s="17" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="112" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>489</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="F70" s="17" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="96" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>490</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="F71" s="17" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="81" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>491</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="F72" s="17" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="65" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>492</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="F73" s="17" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>493</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="F74" s="17" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="C75" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="F75" s="17" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>495</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="F76" s="17" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="F77" s="17" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>497</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="F78" s="17" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>498</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F79" s="17" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="F80" s="17" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>500</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="F81" s="17" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="48" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>501</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="F82" s="17" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>502</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="F83" s="17" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C84" s="16" t="s">
+        <v>503</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="F84" s="17" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C85" s="15" t="s">
+        <v>504</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="F85" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="64" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="C86" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="F86" s="17" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="401" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>543</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>505</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="F87" s="17" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>506</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="F88" s="17" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>507</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="F89" s="17" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="C90" s="15" t="s">
+        <v>508</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="F90" s="17" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="177" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>542</v>
+      </c>
+      <c r="C91" s="16" t="s">
+        <v>509</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="E91" s="6" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>449</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="320" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>450</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="368" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>451</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>452</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>453</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="409" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>454</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>455</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>456</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="304" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>457</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="368" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>458</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>459</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>460</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="F37" s="17" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>461</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="192" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>462</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="384" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="224" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="409" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>463</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="F42" s="17" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="176" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>464</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="400" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>465</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>466</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="304" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
-        <v>550</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>468</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="F48" s="17" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>470</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="F49" s="17" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="409" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>471</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="F50" s="17" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="304" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>472</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="F51" s="17" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="400" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>473</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="F52" s="17" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>474</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="F53" s="17" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>475</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="F54" s="17" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>476</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="F55" s="17" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>477</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="F56" s="17" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C57" s="15" t="s">
-        <v>478</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="F57" s="17" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="409" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B58" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="C58" s="15" t="s">
-        <v>479</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="F58" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="F59" s="17" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>480</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="F60" s="17" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="400" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
-        <v>545</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>546</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>481</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>547</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>548</v>
-      </c>
-      <c r="F61" s="19" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="409" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B62" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>482</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="F62" s="17" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="352" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="C63" s="15" t="s">
-        <v>483</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="F63" s="17" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="409" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B64" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="C64" s="15" t="s">
-        <v>484</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="F64" s="17" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="409" x14ac:dyDescent="0.25">
-      <c r="A65" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B65" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="C65" s="15" t="s">
-        <v>485</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="F65" s="17" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="409" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="B66" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="C66" s="15" t="s">
-        <v>486</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="F66" s="17" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="C67" s="15" t="s">
-        <v>487</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="F67" s="17" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="409" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B68" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="C68" s="15" t="s">
-        <v>488</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="F68" s="17" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B69" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="C69" s="15" t="s">
-        <v>489</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="F69" s="17" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B70" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="C70" s="15" t="s">
-        <v>490</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="F70" s="17" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="409" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="C71" s="15" t="s">
-        <v>491</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="F71" s="17" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B72" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="C72" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="F72" s="17" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="409" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="C73" s="15" t="s">
-        <v>493</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="F73" s="17" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="400" x14ac:dyDescent="0.25">
-      <c r="A74" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B74" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="C74" s="15" t="s">
-        <v>494</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="F74" s="17" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="B75" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="C75" s="15" t="s">
-        <v>495</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="F75" s="17" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A76" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B76" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="C76" s="15" t="s">
-        <v>496</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="F76" s="17" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="A77" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B77" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="C77" s="15" t="s">
-        <v>497</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="F77" s="17" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="A78" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="C78" s="15" t="s">
-        <v>498</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="F78" s="17" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="A79" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B79" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="C79" s="15" t="s">
-        <v>499</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="F79" s="17" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="32" x14ac:dyDescent="0.25">
-      <c r="A80" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="B80" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="C80" s="15" t="s">
-        <v>500</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="F80" s="17" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="A81" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="B81" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="C81" s="15" t="s">
-        <v>501</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="F81" s="17" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="368" x14ac:dyDescent="0.25">
-      <c r="A82" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="B82" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>502</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="F82" s="17" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="192" x14ac:dyDescent="0.25">
-      <c r="A83" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="B83" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="C83" s="15" t="s">
-        <v>503</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="F83" s="17" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="65" x14ac:dyDescent="0.25">
-      <c r="A84" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="B84" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="C84" s="16" t="s">
-        <v>504</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="F84" s="17" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="112" x14ac:dyDescent="0.25">
-      <c r="A85" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B85" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="C85" s="15" t="s">
-        <v>505</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="F85" s="17" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="336" x14ac:dyDescent="0.25">
-      <c r="A86" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B86" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="C86" s="16" t="s">
-        <v>257</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="F86" s="17" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A87" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="B87" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="C87" s="15" t="s">
-        <v>506</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>512</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="F87" s="17" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A88" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="B88" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="C88" s="15" t="s">
-        <v>507</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="F88" s="17" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="49" x14ac:dyDescent="0.25">
-      <c r="A89" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="B89" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="C89" s="15" t="s">
-        <v>508</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="F89" s="17" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="A90" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="B90" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="C90" s="15" t="s">
-        <v>509</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="F90" s="17" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A91" s="9" t="s">
-        <v>428</v>
-      </c>
-      <c r="B91" s="10" t="s">
-        <v>543</v>
-      </c>
-      <c r="C91" s="16" t="s">
-        <v>510</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>513</v>
-      </c>
-      <c r="E91" s="6" t="s">
+      <c r="F91" s="19" t="s">
         <v>541</v>
-      </c>
-      <c r="F91" s="19" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D92" s="13" t="s">
+        <v>513</v>
+      </c>
+      <c r="E92" s="13" t="s">
         <v>514</v>
       </c>
-      <c r="E92" s="13" t="s">
+      <c r="F92" s="11" t="s">
         <v>515</v>
-      </c>
-      <c r="F92" s="11" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B93" s="20" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C93" s="21" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D93" s="22" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E93" s="23" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F93" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B94" s="20" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C94" s="22" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D94" s="22" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E94" s="23" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F94" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B95" s="20" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C95" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D95" s="22" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E95" s="23" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F95" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B96" s="20" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C96" s="22" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D96" s="22" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E96" s="23" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F96" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B97" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C97" s="22" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D97" s="22" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E97" s="23" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F97" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B98" s="20" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C98" s="22" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D98" s="22" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E98" s="23" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F98" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B99" s="20" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C99" s="22" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D99" s="22" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E99" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F99" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B100" s="20" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C100" s="22" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D100" s="22" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E100" s="23" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F100" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="24" t="s">
         <v>599</v>
+      </c>
+      <c r="B101" s="25" t="s">
+        <v>604</v>
+      </c>
+      <c r="C101" s="25" t="s">
+        <v>602</v>
+      </c>
+      <c r="D101" s="25" t="s">
+        <v>601</v>
+      </c>
+      <c r="E101" s="25" t="s">
+        <v>600</v>
+      </c>
+      <c r="F101" s="25" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="B102" t="s">
+        <v>605</v>
+      </c>
+      <c r="C102" s="16" t="s">
+        <v>607</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="F102" s="19" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="24" t="s">
+        <v>611</v>
+      </c>
+      <c r="B103" s="25" t="s">
+        <v>613</v>
+      </c>
+      <c r="C103" s="25" t="s">
+        <v>614</v>
+      </c>
+      <c r="D103" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="E103" s="25" t="s">
+        <v>615</v>
+      </c>
+      <c r="F103" s="25" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="24" t="s">
+        <v>617</v>
+      </c>
+      <c r="B104" s="24" t="s">
+        <v>618</v>
+      </c>
+      <c r="C104" s="26" t="s">
+        <v>619</v>
+      </c>
+      <c r="D104" s="25" t="s">
+        <v>620</v>
+      </c>
+      <c r="E104" s="27" t="s">
+        <v>621</v>
+      </c>
+      <c r="F104" s="25" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="24" t="s">
+        <v>623</v>
+      </c>
+      <c r="B105" s="25" t="s">
+        <v>628</v>
+      </c>
+      <c r="C105" s="25" t="s">
+        <v>627</v>
+      </c>
+      <c r="D105" s="25" t="s">
+        <v>626</v>
+      </c>
+      <c r="E105" s="25" t="s">
+        <v>625</v>
+      </c>
+      <c r="F105" s="25" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A106" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="C106" s="16" t="s">
+        <v>631</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>633</v>
+      </c>
+      <c r="F106" s="19" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="24" t="s">
+        <v>635</v>
+      </c>
+      <c r="B107" s="25" t="s">
+        <v>636</v>
+      </c>
+      <c r="C107" s="25" t="s">
+        <v>637</v>
+      </c>
+      <c r="D107" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="E107" s="25" t="s">
+        <v>641</v>
+      </c>
+      <c r="F107" s="25" t="s">
+        <v>639</v>
       </c>
     </row>
   </sheetData>

</xml_diff>